<commit_message>
Componer el diagrama de Gantt
</commit_message>
<xml_diff>
--- a/juandadiagrama_gantt_proyecto_gestor_encuestas.xlsx
+++ b/juandadiagrama_gantt_proyecto_gestor_encuestas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ENCUESTA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Programming\Visual Studio Code\Web Development\Analisis y Diseño de Sistemas de Informacion\Encuesta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FFD9355-05E1-4B69-A7EE-D9EC6D3080F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F587B57E-4785-4799-99DB-97D1A2FC5702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagrama Gantt Extendido" sheetId="1" r:id="rId1"/>
@@ -20,62 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Actividad</t>
   </si>
   <si>
-    <t>11/08/2025</t>
-  </si>
-  <si>
-    <t>12/08/2025</t>
-  </si>
-  <si>
-    <t>13/08/2025</t>
-  </si>
-  <si>
-    <t>14/08/2025</t>
-  </si>
-  <si>
-    <t>15/08/2025</t>
-  </si>
-  <si>
-    <t>16/08/2025</t>
-  </si>
-  <si>
-    <t>17/08/2025</t>
-  </si>
-  <si>
-    <t>18/08/2025</t>
-  </si>
-  <si>
-    <t>19/08/2025</t>
-  </si>
-  <si>
-    <t>20/08/2025</t>
-  </si>
-  <si>
-    <t>21/08/2025</t>
-  </si>
-  <si>
-    <t>22/08/2025</t>
-  </si>
-  <si>
-    <t>23/08/2025</t>
-  </si>
-  <si>
-    <t>24/08/2025</t>
-  </si>
-  <si>
-    <t>25/08/2025</t>
-  </si>
-  <si>
-    <t>26/08/2025</t>
-  </si>
-  <si>
-    <t>27/08/2025</t>
-  </si>
-  <si>
     <t>Planificación general y diseño de mockups</t>
   </si>
   <si>
@@ -116,6 +65,30 @@
   </si>
   <si>
     <t>Entrega final</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
   </si>
 </sst>
 </file>
@@ -157,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -300,11 +273,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,7 +300,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,6 +319,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,115 +626,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.5546875" customWidth="1"/>
-    <col min="2" max="18" width="12" customWidth="1"/>
-    <col min="19" max="19" width="10.88671875" customWidth="1"/>
+    <col min="2" max="19" width="2.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="15"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="14">
-        <v>45902</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="5"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -758,20 +752,19 @@
       <c r="R3" s="1"/>
       <c r="S3" s="5"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -781,21 +774,21 @@
       <c r="R4" s="1"/>
       <c r="S4" s="5"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -804,21 +797,20 @@
       <c r="R5" s="1"/>
       <c r="S5" s="5"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -827,22 +819,22 @@
       <c r="R6" s="1"/>
       <c r="S6" s="5"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -850,17 +842,17 @@
       <c r="R7" s="1"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -873,9 +865,9 @@
       <c r="R8" s="1"/>
       <c r="S8" s="5"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -883,12 +875,12 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="2"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -896,9 +888,9 @@
       <c r="R9" s="1"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -907,21 +899,21 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="1"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="2"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="5"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -931,20 +923,20 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="1"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="2"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="5"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -955,19 +947,19 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="2"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -980,7 +972,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="2"/>
       <c r="P13" s="1"/>
@@ -988,9 +980,9 @@
       <c r="R13" s="1"/>
       <c r="S13" s="5"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1004,58 +996,67 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="2"/>
       <c r="R14" s="1"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="10"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:P1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>